<commit_message>
Add calculation of dates for the example file example_resource_plan
</commit_message>
<xml_diff>
--- a/budgeteer-resourceplan-importer/src/main/resources/example_resource_plan.xlsx
+++ b/budgeteer-resourceplan-importer/src/main/resources/example_resource_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trzpiot\Documents\Workspace\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trzpiot\Documents\Workspace\budgeteer\budgeteer-resourceplan-importer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -438,163 +438,163 @@
       </c>
       <c r="F1" s="3">
         <f t="shared" ref="F1:O1" ca="1" si="0">G1-1</f>
-        <v>43283</v>
+        <v>43293</v>
       </c>
       <c r="G1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43284</v>
+        <v>43294</v>
       </c>
       <c r="H1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43285</v>
+        <v>43295</v>
       </c>
       <c r="I1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43286</v>
+        <v>43296</v>
       </c>
       <c r="J1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43287</v>
+        <v>43297</v>
       </c>
       <c r="K1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43288</v>
+        <v>43298</v>
       </c>
       <c r="L1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43289</v>
+        <v>43299</v>
       </c>
       <c r="M1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43290</v>
+        <v>43300</v>
       </c>
       <c r="N1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43291</v>
+        <v>43301</v>
       </c>
       <c r="O1" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>43292</v>
+        <v>43302</v>
       </c>
       <c r="P1" s="3">
         <f t="shared" ref="P1:AQ1" ca="1" si="1">Q1-1</f>
-        <v>43293</v>
+        <v>43303</v>
       </c>
       <c r="Q1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43294</v>
+        <v>43304</v>
       </c>
       <c r="R1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43295</v>
+        <v>43305</v>
       </c>
       <c r="S1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43296</v>
+        <v>43306</v>
       </c>
       <c r="T1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43297</v>
+        <v>43307</v>
       </c>
       <c r="U1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43298</v>
+        <v>43308</v>
       </c>
       <c r="V1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43299</v>
+        <v>43309</v>
       </c>
       <c r="W1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43300</v>
+        <v>43310</v>
       </c>
       <c r="X1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43301</v>
+        <v>43311</v>
       </c>
       <c r="Y1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43302</v>
+        <v>43312</v>
       </c>
       <c r="Z1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43303</v>
+        <v>43313</v>
       </c>
       <c r="AA1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43304</v>
+        <v>43314</v>
       </c>
       <c r="AB1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43305</v>
+        <v>43315</v>
       </c>
       <c r="AC1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43306</v>
+        <v>43316</v>
       </c>
       <c r="AD1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43307</v>
+        <v>43317</v>
       </c>
       <c r="AE1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43308</v>
+        <v>43318</v>
       </c>
       <c r="AF1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43309</v>
+        <v>43319</v>
       </c>
       <c r="AG1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43310</v>
+        <v>43320</v>
       </c>
       <c r="AH1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43311</v>
+        <v>43321</v>
       </c>
       <c r="AI1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43312</v>
+        <v>43322</v>
       </c>
       <c r="AJ1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43313</v>
+        <v>43323</v>
       </c>
       <c r="AK1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43314</v>
+        <v>43324</v>
       </c>
       <c r="AL1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43315</v>
+        <v>43325</v>
       </c>
       <c r="AM1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43316</v>
+        <v>43326</v>
       </c>
       <c r="AN1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43317</v>
+        <v>43327</v>
       </c>
       <c r="AO1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43318</v>
+        <v>43328</v>
       </c>
       <c r="AP1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43319</v>
+        <v>43329</v>
       </c>
       <c r="AQ1" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43320</v>
+        <v>43330</v>
       </c>
       <c r="AR1" s="3">
         <f ca="1">AS1-1</f>
-        <v>43321</v>
+        <v>43331</v>
       </c>
       <c r="AS1" s="3">
         <f ca="1">TODAY()</f>
-        <v>43322</v>
+        <v>43332</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.3">
@@ -608,12 +608,12 @@
         <v>500</v>
       </c>
       <c r="D2" s="1">
-        <f ca="1">SUM(P2:AS2)</f>
-        <v>176</v>
+        <f ca="1">SUM(F2:AS2)</f>
+        <v>224</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">D2*C2/8</f>
-        <v>11000</v>
+        <v>14000</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:AR2" ca="1" si="2">IF(OR(WEEKDAY(F1,2)=6,WEEKDAY(F1,2)=7),0,8)</f>
@@ -625,11 +625,11 @@
       </c>
       <c r="H2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -637,11 +637,11 @@
       </c>
       <c r="K2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -653,11 +653,11 @@
       </c>
       <c r="O2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -665,11 +665,11 @@
       </c>
       <c r="R2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -681,11 +681,11 @@
       </c>
       <c r="V2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="X2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -693,11 +693,11 @@
       </c>
       <c r="Y2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -709,11 +709,11 @@
       </c>
       <c r="AC2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -721,11 +721,11 @@
       </c>
       <c r="AF2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -737,11 +737,11 @@
       </c>
       <c r="AJ2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AK2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AL2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -749,11 +749,11 @@
       </c>
       <c r="AM2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AN2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AO2" s="1">
         <f t="shared" ca="1" si="2"/>
@@ -765,11 +765,11 @@
       </c>
       <c r="AQ2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AR2" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AS2" s="1">
         <f ca="1">IF(OR(WEEKDAY(AS1,2)=6,WEEKDAY(AS1,2)=7),0,8)</f>
@@ -787,12 +787,12 @@
         <v>1000</v>
       </c>
       <c r="D3" s="1">
-        <f ca="1">SUM(P3:AS3)</f>
-        <v>88</v>
+        <f ca="1">SUM(F3:AS3)</f>
+        <v>112</v>
       </c>
       <c r="E3" s="1">
         <f ca="1">D3*C3/8</f>
-        <v>11000</v>
+        <v>14000</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:AR3" ca="1" si="3">IF(OR(WEEKDAY(F1,2)=6,WEEKDAY(F1,2)=7),0,4)</f>
@@ -804,11 +804,11 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -816,11 +816,11 @@
       </c>
       <c r="K3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -832,11 +832,11 @@
       </c>
       <c r="O3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -844,11 +844,11 @@
       </c>
       <c r="R3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -860,11 +860,11 @@
       </c>
       <c r="V3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="X3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -872,11 +872,11 @@
       </c>
       <c r="Y3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -888,11 +888,11 @@
       </c>
       <c r="AC3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AD3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -900,11 +900,11 @@
       </c>
       <c r="AF3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -916,11 +916,11 @@
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AL3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -928,11 +928,11 @@
       </c>
       <c r="AM3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AO3" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -944,11 +944,11 @@
       </c>
       <c r="AQ3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AR3" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AS3" s="1">
         <f ca="1">IF(OR(WEEKDAY(AS1,2)=6,WEEKDAY(AS1,2)=7),0,4)</f>

</xml_diff>